<commit_message>
-Added an 'Other' row in the budget
Former-commit-id: a694b8f8836d8a926fa7abb04f83072d005f6ca6
</commit_message>
<xml_diff>
--- a/data/TechWorkshop.xlsx
+++ b/data/TechWorkshop.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>GlycoNet Tech Workshops Budget</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Lunch and snacks:</t>
+  </si>
+  <si>
+    <t>Other:</t>
   </si>
   <si>
     <t>SUPPLIES &amp; RESOURCES TOTAL:</t>
@@ -333,10 +336,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -466,48 +469,48 @@
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="n">
-        <f aca="false">SUM(B9:B13)</f>
-        <v>0</v>
-      </c>
+      <c r="B14" s="7"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="7" t="n">
+        <f aca="false">SUM(B9:B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
@@ -531,44 +534,53 @@
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7" t="n">
-        <f aca="false">SUM(B17:B19)</f>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="n">
+        <f aca="false">SUM(B18:B20)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="7" t="n">
-        <f aca="false">SUM(C17:C19)</f>
+      <c r="C21" s="7" t="n">
+        <f aca="false">SUM(C18:C20)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="7" t="n">
-        <f aca="false">SUM(D17:D19)</f>
+      <c r="D21" s="7" t="n">
+        <f aca="false">SUM(D18:D20)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="7" t="n">
-        <f aca="false">SUM(E17:E19)</f>
+      <c r="E21" s="7" t="n">
+        <f aca="false">SUM(E18:E20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-    </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="7" t="n">
-        <f aca="false">SUM(B20:E20,B14)</f>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="7" t="n">
+        <f aca="false">SUM(B21:E21,B15)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
@@ -582,8 +594,9 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="C23:E23"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
-Added the Regional Meeting application
Former-commit-id: 876c41735701821b0817ee22e27e23f2d3dff8d1
</commit_message>
<xml_diff>
--- a/data/TechWorkshop.xlsx
+++ b/data/TechWorkshop.xlsx
@@ -210,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,40 +223,48 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -339,7 +347,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -388,13 +396,13 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3"/>
@@ -403,112 +411,112 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="8" t="n">
         <f aca="false">SUM(B9:B14)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -516,68 +524,68 @@
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="8" t="n">
         <f aca="false">SUM(B18:B20)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="8" t="n">
         <f aca="false">SUM(C18:C20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D21" s="8" t="n">
         <f aca="false">SUM(D18:D20)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="E21" s="8" t="n">
         <f aca="false">SUM(E18:E20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="7" t="n">
+      <c r="B23" s="8" t="n">
         <f aca="false">SUM(B21:E21,B15)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
-Changed the glyconet budget template
Former-commit-id: 473f6ab6c28fa936f1be682758ca70a3d25a7d43
</commit_message>
<xml_diff>
--- a/data/TechWorkshop.xlsx
+++ b/data/TechWorkshop.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>GlycoNet Tech Workshops Budget</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Accommodations:</t>
-  </si>
-  <si>
-    <t>Honoraria (non-GlycoNet only):</t>
   </si>
   <si>
     <t>FACILITATOR TOTAL:</t>
@@ -344,10 +341,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -542,50 +539,41 @@
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="B20" s="8" t="n">
+        <f aca="false">SUM(B18:B19)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="n">
+        <f aca="false">SUM(C18:C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <f aca="false">SUM(D18:D19)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="8" t="n">
+        <f aca="false">SUM(E18:E19)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="8" t="n">
-        <f aca="false">SUM(B18:B20)</f>
+      <c r="B22" s="8" t="n">
+        <f aca="false">SUM(B20:E20,B15)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="8" t="n">
-        <f aca="false">SUM(C18:C20)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="8" t="n">
-        <f aca="false">SUM(D18:D20)</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="8" t="n">
-        <f aca="false">SUM(E18:E20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="8" t="n">
-        <f aca="false">SUM(B21:E21,B15)</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -604,7 +592,7 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>